<commit_message>
Update for all other PCs
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8037EB1-B8A7-4F2E-9FF9-34C833FD7AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4480696C-2362-46B2-8795-C3ACAEF3D555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12915" yWindow="3990" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adjustement to mace and justification
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F77F3B-1D79-4850-9128-4A38DDB4A76F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12026A10-7FFC-4706-89D9-859597F9AADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12915" yWindow="3990" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="33">
   <si>
     <t>adult</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>Full runs completed</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Run not possible / Too long</t>
   </si>
 </sst>
 </file>
@@ -133,7 +139,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -152,6 +158,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -165,10 +177,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A5DD07-537B-4123-974E-B57E61B97201}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,8 +795,8 @@
       <c r="H8" t="s">
         <v>28</v>
       </c>
-      <c r="I8" t="s">
-        <v>27</v>
+      <c r="I8" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="J8" t="s">
         <v>28</v>
@@ -1100,14 +1113,20 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="3"/>
       <c r="B18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Upload results corrected eval
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E4069D-5E10-4DA9-A306-AC522B4CE667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B1D231-2465-4069-BCC3-8CEB60539998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="4125" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
+    <workbookView xWindow="16380" yWindow="4515" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -490,7 +490,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,22 +549,22 @@
       <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -587,22 +587,22 @@
       <c r="E3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="J3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L3" s="2" t="s">
@@ -625,22 +625,22 @@
       <c r="E4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="F4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="J4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L4" s="2" t="s">
@@ -663,22 +663,22 @@
       <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="F5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" t="s">
+      <c r="J5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L5" s="2" t="s">
@@ -701,25 +701,25 @@
       <c r="E6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="J6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -739,10 +739,10 @@
       <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="F7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H7" t="s">
@@ -757,7 +757,7 @@
       <c r="K7" t="s">
         <v>25</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -795,7 +795,7 @@
       <c r="K8" t="s">
         <v>25</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -833,7 +833,7 @@
       <c r="K9" t="s">
         <v>25</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -871,7 +871,7 @@
       <c r="K10" t="s">
         <v>25</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -909,7 +909,7 @@
       <c r="K11" t="s">
         <v>25</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -947,7 +947,7 @@
       <c r="K12" t="s">
         <v>25</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -985,7 +985,7 @@
       <c r="K13" t="s">
         <v>25</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       <c r="K14" t="s">
         <v>25</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       <c r="K15" t="s">
         <v>25</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Running all datasets except diabetes Home
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B1D231-2465-4069-BCC3-8CEB60539998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B511F3-0D6E-4358-8DD4-27ADB63CB8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16380" yWindow="4515" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -745,16 +745,16 @@
       <c r="G7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" t="s">
+      <c r="J7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L7" s="2" t="s">
@@ -789,7 +789,7 @@
       <c r="I8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K8" t="s">
@@ -827,7 +827,7 @@
       <c r="I9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K9" t="s">
@@ -865,7 +865,7 @@
       <c r="I10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K10" t="s">
@@ -903,7 +903,7 @@
       <c r="I11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K11" t="s">
@@ -941,7 +941,7 @@
       <c r="I12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K12" t="s">
@@ -979,7 +979,7 @@
       <c r="I13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K13" t="s">
@@ -1017,7 +1017,7 @@
       <c r="I14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J14" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K14" t="s">
@@ -1055,7 +1055,7 @@
       <c r="I15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J15" s="3" t="s">
         <v>25</v>
       </c>
       <c r="K15" t="s">

</xml_diff>

<commit_message>
Missing diabetes and CCHVAE
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B511F3-0D6E-4358-8DD4-27ADB63CB8FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF9381B-5185-45FC-A535-6766691EF768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
@@ -490,7 +490,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,13 +777,13 @@
       <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="F8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I8" s="2" t="s">
@@ -792,7 +792,7 @@
       <c r="J8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L8" s="2" t="s">
@@ -853,13 +853,13 @@
       <c r="E10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="F10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -868,7 +868,7 @@
       <c r="J10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L10" s="2" t="s">
@@ -891,13 +891,13 @@
       <c r="E11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="F11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I11" s="2" t="s">
@@ -906,7 +906,7 @@
       <c r="J11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L11" s="2" t="s">
@@ -929,13 +929,13 @@
       <c r="E12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="F12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I12" s="2" t="s">
@@ -944,7 +944,7 @@
       <c r="J12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L12" s="2" t="s">
@@ -967,13 +967,13 @@
       <c r="E13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="F13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -982,7 +982,7 @@
       <c r="J13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L13" s="2" t="s">
@@ -1005,13 +1005,13 @@
       <c r="E14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="F14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -1020,7 +1020,7 @@
       <c r="J14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L14" s="2" t="s">
@@ -1043,13 +1043,13 @@
       <c r="E15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" t="s">
-        <v>25</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="F15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I15" s="2" t="s">
@@ -1058,7 +1058,7 @@
       <c r="J15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L15" s="2" t="s">

</xml_diff>

<commit_message>
CCHVAE Progress. Credit and Student requiring more test
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF9381B-5185-45FC-A535-6766691EF768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D73FF9-95BD-4164-8B2D-AC581FEC4084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
+    <workbookView xWindow="8235" yWindow="4680" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,7 +713,7 @@
       <c r="I6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="3" t="s">
+      <c r="J6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K6" s="2" t="s">
@@ -789,7 +789,7 @@
       <c r="I8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K8" s="2" t="s">
@@ -815,13 +815,13 @@
       <c r="E9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -830,7 +830,7 @@
       <c r="J9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="L9" s="2" t="s">

</xml_diff>

<commit_message>
Fixing Extra tests. Run exp. Ubuntu: Adult, census, german, dutch, bank
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D6502C-6F69-4941-9EF0-66056F507F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC567901-EF79-4012-9638-2F3C0B5927C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8235" yWindow="4680" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
+    <workbookView xWindow="18675" yWindow="4065" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="31">
   <si>
     <t>adult</t>
   </si>
@@ -115,14 +115,25 @@
   </si>
   <si>
     <t>Run not possible / Too long</t>
+  </si>
+  <si>
+    <t>EXTRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -168,11 +179,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -479,7 +492,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -487,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A5DD07-537B-4123-974E-B57E61B97201}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,25 +1078,596 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L29" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
credit done MACE extra
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC567901-EF79-4012-9638-2F3C0B5927C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64679B77-DA22-4F8F-AD07-1CF3A8611534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18675" yWindow="4065" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
@@ -179,13 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +502,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,37 +1137,37 @@
       <c r="A22" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" s="5" t="s">
+      <c r="B22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
         <v>25</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K22" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L22" s="5" t="s">
+      <c r="J22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1176,37 +1175,37 @@
       <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" s="5" t="s">
+      <c r="B23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" t="s">
         <v>25</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" s="5" t="s">
+      <c r="J23" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1214,37 +1213,37 @@
       <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="5" t="s">
+      <c r="B24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" t="s">
         <v>25</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24" s="5" t="s">
+      <c r="J24" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1252,37 +1251,37 @@
       <c r="A25" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="5" t="s">
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
         <v>25</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L25" s="5" t="s">
+      <c r="J25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1290,37 +1289,37 @@
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="5" t="s">
+      <c r="B26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" t="s">
         <v>25</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L26" s="5" t="s">
+      <c r="J26" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1328,37 +1327,37 @@
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K27" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L27" s="5" t="s">
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+      <c r="K27" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1366,37 +1365,37 @@
       <c r="A28" t="s">
         <v>6</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L28" s="5" t="s">
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1404,37 +1403,37 @@
       <c r="A29" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L29" s="5" t="s">
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" t="s">
+        <v>25</v>
+      </c>
+      <c r="K29" t="s">
+        <v>25</v>
+      </c>
+      <c r="L29" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1442,37 +1441,37 @@
       <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L30" s="5" t="s">
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" t="s">
+        <v>25</v>
+      </c>
+      <c r="K30" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1480,37 +1479,37 @@
       <c r="A31" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K31" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L31" s="5" t="s">
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" t="s">
+        <v>25</v>
+      </c>
+      <c r="J31" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1518,37 +1517,37 @@
       <c r="A32" t="s">
         <v>10</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L32" s="5" t="s">
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32" t="s">
+        <v>25</v>
+      </c>
+      <c r="K32" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1556,37 +1555,37 @@
       <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L33" s="5" t="s">
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K33" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1594,37 +1593,37 @@
       <c r="A34" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L34" s="5" t="s">
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" t="s">
+        <v>25</v>
+      </c>
+      <c r="K34" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1632,37 +1631,37 @@
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="L35" s="5" t="s">
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" t="s">
+        <v>25</v>
+      </c>
+      <c r="K35" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Running compas still (halfway)
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64679B77-DA22-4F8F-AD07-1CF3A8611534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F3FDFC-4FFF-4782-A81C-BD947B7FDF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18675" yWindow="4065" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A5DD07-537B-4123-974E-B57E61B97201}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,16 +1327,16 @@
       <c r="A27" t="s">
         <v>5</v>
       </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
-      </c>
-      <c r="D27" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="B27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F27" t="s">
@@ -1631,16 +1631,16 @@
       <c r="A35" t="s">
         <v>13</v>
       </c>
-      <c r="B35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" t="s">
-        <v>26</v>
-      </c>
-      <c r="D35" t="s">
-        <v>26</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="B35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F35" t="s">

</xml_diff>

<commit_message>
Ready for NN, MO, FT, RT for all except diabetes
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F3FDFC-4FFF-4782-A81C-BD947B7FDF67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2958DB33-4859-431C-BAE2-E3D8FDF6270F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18675" yWindow="4065" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
@@ -502,7 +502,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N27" sqref="N27"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1386,7 +1386,7 @@
       <c r="H28" t="s">
         <v>25</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J28" t="s">
@@ -1462,7 +1462,7 @@
       <c r="H30" t="s">
         <v>25</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J30" t="s">
@@ -1500,7 +1500,7 @@
       <c r="H31" t="s">
         <v>25</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J31" t="s">
@@ -1538,7 +1538,7 @@
       <c r="H32" t="s">
         <v>25</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J32" t="s">
@@ -1576,7 +1576,7 @@
       <c r="H33" t="s">
         <v>25</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J33" t="s">
@@ -1614,7 +1614,7 @@
       <c r="H34" t="s">
         <v>25</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J34" t="s">
@@ -1652,7 +1652,7 @@
       <c r="H35" t="s">
         <v>25</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="2" t="s">
         <v>25</v>
       </c>
       <c r="J35" t="s">

</xml_diff>

<commit_message>
Missing heart for NN, MO, FT RT, running now
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2958DB33-4859-431C-BAE2-E3D8FDF6270F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEC3DAE-A4AD-4088-A198-CA17F3A166D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18675" yWindow="4065" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
+    <workbookView xWindow="930" yWindow="2730" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -179,12 +179,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,7 +503,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,13 +1150,13 @@
       <c r="E22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="F22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I22" s="2" t="s">
@@ -1164,10 +1165,10 @@
       <c r="J22" t="s">
         <v>25</v>
       </c>
-      <c r="K22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L22" t="s">
+      <c r="K22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1187,13 +1188,13 @@
       <c r="E23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="F23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I23" s="2" t="s">
@@ -1202,10 +1203,10 @@
       <c r="J23" t="s">
         <v>25</v>
       </c>
-      <c r="K23" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" t="s">
+      <c r="K23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1225,13 +1226,13 @@
       <c r="E24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="F24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I24" s="2" t="s">
@@ -1240,10 +1241,10 @@
       <c r="J24" t="s">
         <v>25</v>
       </c>
-      <c r="K24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24" t="s">
+      <c r="K24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1263,13 +1264,13 @@
       <c r="E25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="F25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I25" s="2" t="s">
@@ -1278,10 +1279,10 @@
       <c r="J25" t="s">
         <v>25</v>
       </c>
-      <c r="K25" t="s">
-        <v>25</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="K25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1301,13 +1302,13 @@
       <c r="E26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F26" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="F26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I26" s="2" t="s">
@@ -1316,10 +1317,10 @@
       <c r="J26" t="s">
         <v>25</v>
       </c>
-      <c r="K26" t="s">
-        <v>25</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="K26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1339,13 +1340,13 @@
       <c r="E27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F27" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="F27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I27" s="2" t="s">
@@ -1354,10 +1355,10 @@
       <c r="J27" t="s">
         <v>25</v>
       </c>
-      <c r="K27" t="s">
-        <v>25</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="K27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1365,25 +1366,25 @@
       <c r="A28" t="s">
         <v>6</v>
       </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" t="s">
-        <v>26</v>
-      </c>
-      <c r="F28" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="B28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I28" s="2" t="s">
@@ -1392,10 +1393,10 @@
       <c r="J28" t="s">
         <v>25</v>
       </c>
-      <c r="K28" t="s">
-        <v>25</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="K28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L28" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1403,16 +1404,16 @@
       <c r="A29" t="s">
         <v>7</v>
       </c>
-      <c r="B29" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="B29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F29" t="s">
@@ -1441,25 +1442,25 @@
       <c r="A30" t="s">
         <v>8</v>
       </c>
-      <c r="B30" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" t="s">
-        <v>26</v>
-      </c>
-      <c r="D30" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="B30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I30" s="2" t="s">
@@ -1468,10 +1469,10 @@
       <c r="J30" t="s">
         <v>25</v>
       </c>
-      <c r="K30" t="s">
-        <v>25</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="K30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1479,25 +1480,25 @@
       <c r="A31" t="s">
         <v>9</v>
       </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="B31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I31" s="2" t="s">
@@ -1506,10 +1507,10 @@
       <c r="J31" t="s">
         <v>25</v>
       </c>
-      <c r="K31" t="s">
-        <v>25</v>
-      </c>
-      <c r="L31" t="s">
+      <c r="K31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L31" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1517,25 +1518,25 @@
       <c r="A32" t="s">
         <v>10</v>
       </c>
-      <c r="B32" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" t="s">
-        <v>26</v>
-      </c>
-      <c r="D32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" t="s">
-        <v>26</v>
-      </c>
-      <c r="F32" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="B32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I32" s="2" t="s">
@@ -1544,10 +1545,10 @@
       <c r="J32" t="s">
         <v>25</v>
       </c>
-      <c r="K32" t="s">
-        <v>25</v>
-      </c>
-      <c r="L32" t="s">
+      <c r="K32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1555,25 +1556,25 @@
       <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="B33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="B33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I33" s="2" t="s">
@@ -1582,10 +1583,10 @@
       <c r="J33" t="s">
         <v>25</v>
       </c>
-      <c r="K33" t="s">
-        <v>25</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="K33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1593,25 +1594,25 @@
       <c r="A34" t="s">
         <v>12</v>
       </c>
-      <c r="B34" t="s">
-        <v>26</v>
-      </c>
-      <c r="C34" t="s">
-        <v>26</v>
-      </c>
-      <c r="D34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="B34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I34" s="2" t="s">
@@ -1620,10 +1621,10 @@
       <c r="J34" t="s">
         <v>25</v>
       </c>
-      <c r="K34" t="s">
-        <v>25</v>
-      </c>
-      <c r="L34" t="s">
+      <c r="K34" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1643,13 +1644,13 @@
       <c r="E35" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F35" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="F35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I35" s="2" t="s">
@@ -1658,10 +1659,10 @@
       <c r="J35" t="s">
         <v>25</v>
       </c>
-      <c r="K35" t="s">
-        <v>25</v>
-      </c>
-      <c r="L35" t="s">
+      <c r="K35" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L35" s="2" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding gridsearch on diabetes again
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BEC3DAE-A4AD-4088-A198-CA17F3A166D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B50FB21-D522-4665-8B22-4EF1CF4C6D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="930" yWindow="2730" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
@@ -179,13 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +502,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1226,16 +1225,16 @@
       <c r="E24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="2" t="s">
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" t="s">
         <v>25</v>
       </c>
       <c r="J24" t="s">
@@ -1264,16 +1263,16 @@
       <c r="E25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" s="2" t="s">
+      <c r="F25" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" t="s">
         <v>25</v>
       </c>
       <c r="J25" t="s">
@@ -1302,16 +1301,16 @@
       <c r="E26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="2" t="s">
+      <c r="F26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" t="s">
         <v>25</v>
       </c>
       <c r="J26" t="s">
@@ -1320,7 +1319,7 @@
       <c r="K26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="L26" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1340,16 +1339,16 @@
       <c r="E27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I27" s="2" t="s">
+      <c r="F27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" t="s">
         <v>25</v>
       </c>
       <c r="J27" t="s">
@@ -1358,7 +1357,7 @@
       <c r="K27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L27" s="2" t="s">
+      <c r="L27" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1378,16 +1377,16 @@
       <c r="E28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I28" s="2" t="s">
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" t="s">
         <v>25</v>
       </c>
       <c r="J28" t="s">
@@ -1404,16 +1403,16 @@
       <c r="A29" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" t="s">
         <v>26</v>
       </c>
       <c r="F29" t="s">
@@ -1454,16 +1453,16 @@
       <c r="E30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I30" s="2" t="s">
+      <c r="F30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" t="s">
+        <v>25</v>
+      </c>
+      <c r="I30" t="s">
         <v>25</v>
       </c>
       <c r="J30" t="s">
@@ -1492,16 +1491,16 @@
       <c r="E31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="2" t="s">
+      <c r="F31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" t="s">
         <v>25</v>
       </c>
       <c r="J31" t="s">
@@ -1530,16 +1529,16 @@
       <c r="E32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" s="2" t="s">
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" t="s">
         <v>25</v>
       </c>
       <c r="J32" t="s">
@@ -1556,28 +1555,28 @@
       <c r="A33" t="s">
         <v>11</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I33" s="2" t="s">
+      <c r="B33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" t="s">
+        <v>25</v>
+      </c>
+      <c r="H33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" t="s">
         <v>25</v>
       </c>
       <c r="J33" t="s">
@@ -1606,16 +1605,16 @@
       <c r="E34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I34" s="2" t="s">
+      <c r="F34" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" t="s">
+        <v>25</v>
+      </c>
+      <c r="H34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" t="s">
         <v>25</v>
       </c>
       <c r="J34" t="s">
@@ -1644,16 +1643,16 @@
       <c r="E35" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" s="2" t="s">
+      <c r="F35" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" t="s">
+        <v>25</v>
+      </c>
+      <c r="H35" t="s">
+        <v>25</v>
+      </c>
+      <c r="I35" t="s">
         <v>25</v>
       </c>
       <c r="J35" t="s">

</xml_diff>

<commit_message>
Finished CCHVAE files extras
</commit_message>
<xml_diff>
--- a/computing_distro.xlsx
+++ b/computing_distro.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleja\Documents\GitHub\iJUICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D612FFAB-0D58-4CA0-8441-62D21A24D13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89B553E-D00E-498A-935B-7D55B31B7535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38190" yWindow="5805" windowWidth="16410" windowHeight="15360" xr2:uid="{53A8DE12-3761-4AB5-B746-B5BEB05BFE99}"/>
   </bookViews>
@@ -502,7 +502,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1275,7 +1275,7 @@
       <c r="I25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -1313,7 +1313,7 @@
       <c r="I26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J26" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K26" s="2" t="s">
@@ -1351,7 +1351,7 @@
       <c r="I27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K27" s="2" t="s">
@@ -1389,7 +1389,7 @@
       <c r="I28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J28" s="2" t="s">
         <v>25</v>
       </c>
       <c r="K28" s="2" t="s">

</xml_diff>